<commit_message>
Commit project, on repository
</commit_message>
<xml_diff>
--- a/Le_probleme_des_trois_corps.xlsx
+++ b/Le_probleme_des_trois_corps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cvmqc-my.sharepoint.com/personal/e_aidiallo_etu_cvm_qc_ca/Documents/Documents/Outils de Gestion/Excel/Projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{E9F36288-786F-4DF7-B278-03DFD76960B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A142F3C-4177-428B-A8D3-4543C713F7FC}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{E9F36288-786F-4DF7-B278-03DFD76960B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E75B842-8711-47EC-AAF1-504C900C056C}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{3A08D00D-5835-448E-96A0-725BF2718FAB}"/>
+    <workbookView xWindow="2310" yWindow="195" windowWidth="21690" windowHeight="12705" xr2:uid="{3A08D00D-5835-448E-96A0-725BF2718FAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>Base de temps</t>
   </si>
@@ -679,108 +679,12 @@
   <si>
     <t>i</t>
   </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,14 +872,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1583,16 +1479,118 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1611,108 +1609,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2037,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9FA13B-9195-4209-A218-EDEBD4862AD0}">
   <dimension ref="C2:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39:I39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,17 +1955,17 @@
         <v>6.2831853071795862</v>
       </c>
     </row>
-    <row r="4" spans="3:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="44" t="s">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C4" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="46"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="80"/>
       <c r="L4" s="35" t="s">
         <v>67</v>
       </c>
@@ -2077,27 +1973,23 @@
       <c r="N4" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>69</v>
-      </c>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2112,29 +2004,23 @@
         <f>L5*M5</f>
         <v>0</v>
       </c>
-      <c r="P5" s="35">
-        <f>COS(N5*H19+H18)</f>
-        <v>0.81319969060892061</v>
-      </c>
-      <c r="Q5" s="35">
-        <f>COS(N5*H19+I18)</f>
-        <v>-0.52478323493092116</v>
-      </c>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="37"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="52">
         <v>0</v>
       </c>
-      <c r="I6" s="49"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2152,20 +2038,20 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
     </row>
-    <row r="7" spans="3:17" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="39" t="s">
+    <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="39"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="61"/>
       <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="50">
+      <c r="H7" s="54">
         <v>2</v>
       </c>
-      <c r="I7" s="50"/>
+      <c r="I7" s="54"/>
       <c r="J7" s="4"/>
       <c r="L7" s="35">
         <v>2</v>
@@ -2178,12 +2064,8 @@
         <f t="shared" si="1"/>
         <v>-1.9151844493627805</v>
       </c>
-      <c r="P7" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="35" t="s">
-        <v>71</v>
-      </c>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="L8" s="35">
@@ -2197,26 +2079,20 @@
         <f t="shared" si="1"/>
         <v>-2.9024796443412004</v>
       </c>
-      <c r="P8" s="35">
-        <f>COS(PI()*H27+H26)</f>
-        <v>0.81319969060839803</v>
-      </c>
-      <c r="Q8" s="35">
-        <f>COS(PI()*H19+I18)</f>
-        <v>-0.52478323493112811</v>
-      </c>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="46"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
       <c r="L9" s="35">
         <v>4</v>
       </c>
@@ -2231,20 +2107,20 @@
       <c r="P9" s="35"/>
       <c r="Q9" s="35"/>
     </row>
-    <row r="10" spans="3:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C10" s="37" t="s">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="65"/>
       <c r="G10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="69">
         <v>1</v>
       </c>
-      <c r="I10" s="51"/>
+      <c r="I10" s="69"/>
       <c r="J10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2259,20 +2135,16 @@
         <f t="shared" si="1"/>
         <v>-4.9364759748920992</v>
       </c>
-      <c r="P10" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q10" s="35" t="s">
-        <v>73</v>
-      </c>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
     </row>
     <row r="11" spans="3:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="37"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="12" t="s">
         <v>13</v>
       </c>
@@ -2296,22 +2168,16 @@
         <f t="shared" si="1"/>
         <v>-5.9831771104645792</v>
       </c>
-      <c r="P11" s="35">
-        <f>COS(PI()*H35+H34)</f>
-        <v>0.15466840618098721</v>
-      </c>
-      <c r="Q11" s="35">
-        <f>COS(PI()*H35+I34)</f>
-        <v>-0.44920511267109242</v>
-      </c>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
     </row>
     <row r="12" spans="3:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="37"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="65"/>
       <c r="G12" s="12" t="s">
         <v>14</v>
       </c>
@@ -2337,12 +2203,12 @@
       </c>
     </row>
     <row r="13" spans="3:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="37"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="12" t="s">
         <v>15</v>
       </c>
@@ -2368,19 +2234,19 @@
       </c>
     </row>
     <row r="14" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="39"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="61"/>
       <c r="G14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="54">
         <v>2500</v>
       </c>
-      <c r="I14" s="50"/>
+      <c r="I14" s="54"/>
       <c r="J14" s="3" t="s">
         <v>32</v>
       </c>
@@ -2410,16 +2276,16 @@
       </c>
     </row>
     <row r="16" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="77"/>
       <c r="L16" s="35">
         <v>11</v>
       </c>
@@ -2433,16 +2299,16 @@
       </c>
     </row>
     <row r="17" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="54"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="74"/>
       <c r="L17" s="35">
         <v>12</v>
       </c>
@@ -2456,12 +2322,12 @@
       </c>
     </row>
     <row r="18" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
       <c r="G18" s="24" t="s">
         <v>35</v>
       </c>
@@ -2487,19 +2353,19 @@
       </c>
     </row>
     <row r="19" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
       <c r="G19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="49">
+      <c r="H19" s="52">
         <v>5000</v>
       </c>
-      <c r="I19" s="49"/>
+      <c r="I19" s="52"/>
       <c r="J19" s="2" t="s">
         <v>32</v>
       </c>
@@ -2516,19 +2382,19 @@
       </c>
     </row>
     <row r="20" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
       <c r="G20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="49">
+      <c r="H20" s="52">
         <v>1</v>
       </c>
-      <c r="I20" s="49"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="2" t="s">
         <v>54</v>
       </c>
@@ -2545,20 +2411,20 @@
       </c>
     </row>
     <row r="21" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="55">
+      <c r="H21" s="42">
         <f>4/3*(PI()*H19^3)</f>
         <v>523598775598.29883</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="8" t="s">
         <v>42</v>
       </c>
@@ -2575,20 +2441,20 @@
       </c>
     </row>
     <row r="22" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="55">
+      <c r="H22" s="42">
         <f>H20*H21</f>
         <v>523598775598.29883</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="8" t="s">
         <v>52</v>
       </c>
@@ -2604,21 +2470,21 @@
         <v>-18.803820294831159</v>
       </c>
     </row>
-    <row r="23" spans="3:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C23" s="56" t="s">
+    <row r="23" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="C23" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="55">
+      <c r="H23" s="42">
         <f>H19*H7</f>
         <v>10000</v>
       </c>
-      <c r="I23" s="55"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="8" t="s">
         <v>32</v>
       </c>
@@ -2635,19 +2501,19 @@
       </c>
     </row>
     <row r="24" spans="3:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="50" t="s">
+      <c r="H24" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="50"/>
+      <c r="I24" s="54"/>
       <c r="J24" s="3"/>
       <c r="L24" s="35">
         <v>19</v>
@@ -2662,16 +2528,16 @@
       </c>
     </row>
     <row r="25" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="59"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="64"/>
       <c r="L25" s="35">
         <v>20</v>
       </c>
@@ -2685,12 +2551,12 @@
       </c>
     </row>
     <row r="26" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
       <c r="G26" s="28" t="s">
         <v>46</v>
       </c>
@@ -2716,19 +2582,19 @@
       </c>
     </row>
     <row r="27" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C27" s="62" t="s">
+      <c r="C27" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="49">
+      <c r="H27" s="52">
         <v>3500</v>
       </c>
-      <c r="I27" s="49"/>
+      <c r="I27" s="52"/>
       <c r="J27" s="2" t="s">
         <v>32</v>
       </c>
@@ -2745,19 +2611,19 @@
       </c>
     </row>
     <row r="28" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="49">
+      <c r="H28" s="52">
         <v>1</v>
       </c>
-      <c r="I28" s="49"/>
+      <c r="I28" s="52"/>
       <c r="J28" s="2" t="s">
         <v>54</v>
       </c>
@@ -2774,20 +2640,20 @@
       </c>
     </row>
     <row r="29" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
       <c r="G29" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H29" s="68">
+      <c r="H29" s="53">
         <f>4/3*(PI()*H27^3)</f>
         <v>179594380030.21649</v>
       </c>
-      <c r="I29" s="68"/>
+      <c r="I29" s="53"/>
       <c r="J29" s="30" t="s">
         <v>53</v>
       </c>
@@ -2804,20 +2670,20 @@
       </c>
     </row>
     <row r="30" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="68">
+      <c r="H30" s="53">
         <f>H28*H29</f>
         <v>179594380030.21649</v>
       </c>
-      <c r="I30" s="68"/>
+      <c r="I30" s="53"/>
       <c r="J30" s="30" t="s">
         <v>18</v>
       </c>
@@ -2834,20 +2700,20 @@
       </c>
     </row>
     <row r="31" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="68">
+      <c r="H31" s="53">
         <f>H27*H7</f>
         <v>7000</v>
       </c>
-      <c r="I31" s="68"/>
+      <c r="I31" s="53"/>
       <c r="J31" s="30" t="s">
         <v>32</v>
       </c>
@@ -2864,19 +2730,19 @@
       </c>
     </row>
     <row r="32" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
       <c r="G32" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="50" t="s">
+      <c r="H32" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="50"/>
+      <c r="I32" s="54"/>
       <c r="J32" s="32"/>
       <c r="L32" s="35">
         <v>27</v>
@@ -2891,16 +2757,16 @@
       </c>
     </row>
     <row r="33" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="70"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="45"/>
       <c r="L33" s="35">
         <v>28</v>
       </c>
@@ -2914,12 +2780,12 @@
       </c>
     </row>
     <row r="34" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C34" s="71" t="s">
+      <c r="C34" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
       <c r="G34" s="16" t="s">
         <v>59</v>
       </c>
@@ -2945,19 +2811,19 @@
       </c>
     </row>
     <row r="35" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
       <c r="G35" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="77">
+      <c r="H35" s="41">
         <v>5000</v>
       </c>
-      <c r="I35" s="77"/>
+      <c r="I35" s="41"/>
       <c r="J35" s="19" t="s">
         <v>32</v>
       </c>
@@ -2974,19 +2840,19 @@
       </c>
     </row>
     <row r="36" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
       <c r="G36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="77">
+      <c r="H36" s="41">
         <v>1</v>
       </c>
-      <c r="I36" s="77"/>
+      <c r="I36" s="41"/>
       <c r="J36" s="19" t="s">
         <v>63</v>
       </c>
@@ -3003,20 +2869,20 @@
       </c>
     </row>
     <row r="37" spans="3:14" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="C37" s="64" t="s">
+      <c r="C37" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H37" s="55">
+      <c r="H37" s="42">
         <f>4/3*(PI()*H35^3)</f>
         <v>523598775598.29883</v>
       </c>
-      <c r="I37" s="55"/>
+      <c r="I37" s="42"/>
       <c r="J37" s="8" t="s">
         <v>64</v>
       </c>
@@ -3033,20 +2899,20 @@
       </c>
     </row>
     <row r="38" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C38" s="64" t="s">
+      <c r="C38" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="55">
+      <c r="H38" s="42">
         <f>H36*H37</f>
         <v>523598775598.29883</v>
       </c>
-      <c r="I38" s="55"/>
+      <c r="I38" s="42"/>
       <c r="J38" s="8" t="s">
         <v>18</v>
       </c>
@@ -3063,20 +2929,20 @@
       </c>
     </row>
     <row r="39" spans="3:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
       <c r="G39" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="55">
+      <c r="H39" s="42">
         <f>H35*H7</f>
         <v>10000</v>
       </c>
-      <c r="I39" s="55"/>
+      <c r="I39" s="42"/>
       <c r="J39" s="8" t="s">
         <v>32</v>
       </c>
@@ -3093,19 +2959,19 @@
       </c>
     </row>
     <row r="40" spans="3:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
       <c r="G40" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="78" t="s">
+      <c r="H40" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="78"/>
+      <c r="I40" s="43"/>
       <c r="J40" s="21"/>
       <c r="L40" s="35">
         <v>35</v>
@@ -3966,44 +3832,10 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C9:J9"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="H5:I5"/>
@@ -4020,10 +3852,44 @@
     <mergeCell ref="C17:J17"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="C38:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4195,18 +4061,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4228,14 +4094,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D003F6E1-D350-4CE5-B436-91C7CDBB608A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEDAC1D7-17AC-4488-BE8B-739AC0DB170D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4249,4 +4107,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D003F6E1-D350-4CE5-B436-91C7CDBB608A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>